<commit_message>
- refactor some codes - add new tables and controllers - a little updates on DB Design
</commit_message>
<xml_diff>
--- a/Documentations/DB Design v1.00.xlsx
+++ b/Documentations/DB Design v1.00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Masters" sheetId="2" r:id="rId1"/>
@@ -319,9 +319,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -330,6 +327,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -622,7 +622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -635,372 +635,372 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4"/>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4"/>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4"/>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4"/>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4"/>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4"/>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4"/>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="4"/>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="4"/>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="4"/>
+      <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="4"/>
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="4"/>
+      <c r="B21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="4"/>
+      <c r="B22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="4"/>
+      <c r="C26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="4"/>
+      <c r="B27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="4"/>
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="4"/>
+      <c r="C29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="4"/>
+      <c r="B30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="4"/>
+      <c r="B31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="4"/>
+      <c r="B32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="4"/>
+      <c r="B33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1016,403 +1016,403 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4"/>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4"/>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4"/>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="F11" s="1" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="F11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="F13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="4"/>
+      <c r="H13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="F14" s="4" t="s">
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="F14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="4" t="s">
+      <c r="H14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="F15" s="4" t="s">
+      <c r="D15" s="3"/>
+      <c r="F15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="4" t="s">
+      <c r="H15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="F16" s="4" t="s">
+      <c r="D16" s="3"/>
+      <c r="F16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="F17" s="4" t="s">
+      <c r="D17" s="3"/>
+      <c r="F17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="4"/>
+      <c r="G17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="F18" s="4" t="s">
+      <c r="D18" s="3"/>
+      <c r="F18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="4"/>
+      <c r="G18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="4"/>
+      <c r="G19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="4"/>
+      <c r="G20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="4"/>
+      <c r="B21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="4"/>
+      <c r="B22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="4"/>
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="4"/>
+      <c r="B24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1423,116 +1423,116 @@
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="4"/>
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="C29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="4"/>
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="4"/>
+      <c r="C31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="4"/>
+      <c r="B32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="4"/>
+      <c r="B33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="4"/>
+      <c r="B34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="4"/>
+      <c r="B35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
@@ -1543,106 +1543,106 @@
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="4"/>
+      <c r="C39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="C40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="C41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="4"/>
+      <c r="B42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="4"/>
+      <c r="B43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="4"/>
+      <c r="B44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="4"/>
+      <c r="B45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1660,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,468 +1673,468 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4"/>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4"/>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4"/>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4"/>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4"/>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="4"/>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="4"/>
+      <c r="C16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="4"/>
+      <c r="C19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="4"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="4"/>
+      <c r="B22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="4"/>
+      <c r="B23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="4"/>
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="4"/>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="4"/>
+      <c r="C29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="4"/>
+      <c r="C32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="4"/>
+      <c r="B33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="C34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="4"/>
+      <c r="C35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="4"/>
+      <c r="C36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="4"/>
+      <c r="B37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="4"/>
+      <c r="B38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="4"/>
+      <c r="B39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="4"/>
+      <c r="B40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>